<commit_message>
Made few changes to the function
</commit_message>
<xml_diff>
--- a/tests/artifact/script/AddProductPage.xlsx
+++ b/tests/artifact/script/AddProductPage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6950" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView windowWidth="18350" windowHeight="6950" tabRatio="500" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="844">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="845">
   <si>
     <t>target</t>
   </si>
@@ -2359,6 +2359,10 @@
   </si>
   <si>
     <t>rowsOfColumn=${columnBusiness}</t>
+  </si>
+  <si>
+    <t>rowsOfColumn=${columnBusiness}
+columnName=${columnName}</t>
   </si>
   <si>
     <t>click on add button in Contact page</t>
@@ -6522,10 +6526,10 @@
   <sheetPr/>
   <dimension ref="A1:O168"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6:E6"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
@@ -9589,10 +9593,10 @@
   <sheetPr/>
   <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
@@ -9855,7 +9859,7 @@
       <c r="N9" s="48"/>
       <c r="O9" s="39"/>
     </row>
-    <row r="10" customFormat="1" ht="29" customHeight="1" spans="1:15">
+    <row r="10" customFormat="1" ht="43.5" spans="1:15">
       <c r="A10" s="26"/>
       <c r="B10" s="21" t="s">
         <v>762</v>
@@ -9870,7 +9874,7 @@
         <v>763</v>
       </c>
       <c r="F10" s="47" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="G10" s="29"/>
       <c r="H10" s="29"/>
@@ -10803,7 +10807,7 @@
   <dimension ref="A1:O90"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
@@ -11071,7 +11075,7 @@
     <row r="10" customFormat="1" ht="29" customHeight="1" spans="1:15">
       <c r="A10" s="26"/>
       <c r="B10" s="21" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="C10" s="28" t="s">
         <v>30</v>
@@ -11080,10 +11084,10 @@
         <v>576</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="F10" s="29" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="G10" s="29"/>
       <c r="H10" s="29"/>
@@ -11097,10 +11101,10 @@
     </row>
     <row r="11" s="3" customFormat="1" ht="65" customHeight="1" spans="1:15">
       <c r="A11" s="20" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="C11" s="31" t="s">
         <v>30</v>
@@ -11109,7 +11113,7 @@
         <v>253</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="F11" s="32"/>
       <c r="G11" s="32"/>
@@ -11125,7 +11129,7 @@
     <row r="12" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A12" s="20"/>
       <c r="B12" s="21" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="C12" s="31" t="s">
         <v>30</v>
@@ -11134,7 +11138,7 @@
         <v>363</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="F12" s="32"/>
       <c r="G12" s="32"/>
@@ -11150,7 +11154,7 @@
     <row r="13" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A13" s="20"/>
       <c r="B13" s="33" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="C13" s="34" t="s">
         <v>30</v>
@@ -11159,7 +11163,7 @@
         <v>253</v>
       </c>
       <c r="E13" s="36" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="F13" s="36"/>
       <c r="G13" s="32"/>
@@ -11175,7 +11179,7 @@
     <row r="14" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A14" s="20"/>
       <c r="B14" s="33" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="C14" s="34" t="s">
         <v>5</v>
@@ -11184,10 +11188,10 @@
         <v>471</v>
       </c>
       <c r="E14" s="36" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="F14" s="36" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="G14" s="32"/>
       <c r="H14" s="32"/>
@@ -11202,7 +11206,7 @@
     <row r="15" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A15" s="20"/>
       <c r="B15" s="33" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="C15" s="34" t="s">
         <v>30</v>
@@ -11211,10 +11215,10 @@
         <v>706</v>
       </c>
       <c r="E15" s="35" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="F15" s="36" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="G15" s="32"/>
       <c r="H15" s="32"/>
@@ -11228,10 +11232,10 @@
     </row>
     <row r="16" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A16" s="20" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="C16" s="31" t="s">
         <v>30</v>
@@ -11240,7 +11244,7 @@
         <v>253</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="F16" s="32"/>
       <c r="G16" s="32"/>
@@ -11256,7 +11260,7 @@
     <row r="17" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A17" s="20"/>
       <c r="B17" s="21" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="C17" s="31" t="s">
         <v>30</v>
@@ -11265,7 +11269,7 @@
         <v>253</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="F17" s="32"/>
       <c r="G17" s="32"/>
@@ -11281,7 +11285,7 @@
     <row r="18" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A18" s="20"/>
       <c r="B18" s="21" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="C18" s="31" t="s">
         <v>30</v>
@@ -11290,10 +11294,10 @@
         <v>707</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="F18" s="32" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="G18" s="32"/>
       <c r="H18" s="32"/>
@@ -11308,7 +11312,7 @@
     <row r="19" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A19" s="20"/>
       <c r="B19" s="21" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="C19" s="31" t="s">
         <v>8</v>
@@ -11317,10 +11321,10 @@
         <v>656</v>
       </c>
       <c r="E19" s="32" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="F19" s="32" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="G19" s="32"/>
       <c r="H19" s="32"/>
@@ -11335,7 +11339,7 @@
     <row r="20" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A20" s="20"/>
       <c r="B20" s="21" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="C20" s="31" t="s">
         <v>30</v>
@@ -11344,7 +11348,7 @@
         <v>253</v>
       </c>
       <c r="E20" s="32" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="F20" s="32"/>
       <c r="G20" s="32"/>
@@ -11360,7 +11364,7 @@
     <row r="21" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A21" s="20"/>
       <c r="B21" s="21" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="C21" s="31" t="s">
         <v>30</v>
@@ -11369,7 +11373,7 @@
         <v>253</v>
       </c>
       <c r="E21" s="32" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="F21" s="35"/>
       <c r="G21" s="32"/>
@@ -11385,7 +11389,7 @@
     <row r="22" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A22" s="20"/>
       <c r="B22" s="21" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="C22" s="31" t="s">
         <v>30</v>
@@ -11394,7 +11398,7 @@
         <v>253</v>
       </c>
       <c r="E22" s="32" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="F22" s="35"/>
       <c r="G22" s="32"/>
@@ -11410,7 +11414,7 @@
     <row r="23" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A23" s="20"/>
       <c r="B23" s="21" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="C23" s="31" t="s">
         <v>30</v>
@@ -11419,10 +11423,10 @@
         <v>707</v>
       </c>
       <c r="E23" s="32" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="F23" s="35" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="G23" s="32"/>
       <c r="H23" s="32"/>
@@ -11437,7 +11441,7 @@
     <row r="24" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A24" s="20"/>
       <c r="B24" s="21" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="C24" s="31" t="s">
         <v>30</v>
@@ -11446,10 +11450,10 @@
         <v>707</v>
       </c>
       <c r="E24" s="32" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="F24" s="35" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="G24" s="32"/>
       <c r="H24" s="32"/>
@@ -11464,7 +11468,7 @@
     <row r="25" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A25" s="20"/>
       <c r="B25" s="21" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="C25" s="31" t="s">
         <v>30</v>
@@ -11473,10 +11477,10 @@
         <v>707</v>
       </c>
       <c r="E25" s="32" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="F25" s="35" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="G25" s="32"/>
       <c r="H25" s="32"/>
@@ -11491,7 +11495,7 @@
     <row r="26" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A26" s="20"/>
       <c r="B26" s="21" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="C26" s="31" t="s">
         <v>30</v>
@@ -11500,7 +11504,7 @@
         <v>253</v>
       </c>
       <c r="E26" s="32" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="F26" s="35"/>
       <c r="G26" s="32"/>
@@ -11515,10 +11519,10 @@
     </row>
     <row r="27" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A27" s="20" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="C27" s="31" t="s">
         <v>30</v>
@@ -11527,7 +11531,7 @@
         <v>253</v>
       </c>
       <c r="E27" s="32" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="F27" s="35"/>
       <c r="G27" s="32"/>
@@ -11543,7 +11547,7 @@
     <row r="28" ht="23" customHeight="1" spans="1:15">
       <c r="A28" s="26"/>
       <c r="B28" s="37" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="C28" s="28" t="s">
         <v>30</v>
@@ -11552,7 +11556,7 @@
         <v>253</v>
       </c>
       <c r="E28" s="29" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="F28" s="29"/>
       <c r="G28" s="29"/>
@@ -11568,7 +11572,7 @@
     <row r="29" ht="23" customHeight="1" spans="1:15">
       <c r="A29" s="26"/>
       <c r="B29" s="37" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="C29" s="28" t="s">
         <v>30</v>
@@ -11577,10 +11581,10 @@
         <v>707</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="F29" s="29" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="G29" s="29"/>
       <c r="H29" s="29"/>
@@ -11595,7 +11599,7 @@
     <row r="30" ht="23" customHeight="1" spans="1:15">
       <c r="A30" s="26"/>
       <c r="B30" s="37" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="C30" s="28" t="s">
         <v>30</v>
@@ -11604,7 +11608,7 @@
         <v>253</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="F30" s="29"/>
       <c r="G30" s="29"/>
@@ -11620,7 +11624,7 @@
     <row r="31" ht="23" customHeight="1" spans="1:15">
       <c r="A31" s="26"/>
       <c r="B31" s="37" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="C31" s="28" t="s">
         <v>30</v>
@@ -11629,10 +11633,10 @@
         <v>707</v>
       </c>
       <c r="E31" s="29" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="F31" s="29" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="G31" s="29"/>
       <c r="H31" s="29"/>
@@ -11647,7 +11651,7 @@
     <row r="32" ht="23" customHeight="1" spans="1:15">
       <c r="A32" s="26"/>
       <c r="B32" s="37" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="C32" s="28" t="s">
         <v>30</v>
@@ -11656,7 +11660,7 @@
         <v>253</v>
       </c>
       <c r="E32" s="29" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="F32" s="29"/>
       <c r="G32" s="29"/>
@@ -11671,10 +11675,10 @@
     </row>
     <row r="33" ht="23" customHeight="1" spans="1:15">
       <c r="A33" s="26" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="B33" s="37" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="C33" s="28" t="s">
         <v>30</v>
@@ -11683,7 +11687,7 @@
         <v>253</v>
       </c>
       <c r="E33" s="29" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="F33" s="29"/>
       <c r="G33" s="29"/>
@@ -11699,7 +11703,7 @@
     <row r="34" ht="23" customHeight="1" spans="1:15">
       <c r="A34" s="26"/>
       <c r="B34" s="37" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="C34" s="28" t="s">
         <v>30</v>
@@ -11708,7 +11712,7 @@
         <v>253</v>
       </c>
       <c r="E34" s="29" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="F34" s="29"/>
       <c r="G34" s="29"/>
@@ -11724,7 +11728,7 @@
     <row r="35" ht="23" customHeight="1" spans="1:15">
       <c r="A35" s="26"/>
       <c r="B35" s="37" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="C35" s="28" t="s">
         <v>30</v>
@@ -11733,7 +11737,7 @@
         <v>253</v>
       </c>
       <c r="E35" s="29" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="F35" s="29"/>
       <c r="G35" s="29"/>
@@ -11749,7 +11753,7 @@
     <row r="36" ht="23" customHeight="1" spans="1:15">
       <c r="A36" s="26"/>
       <c r="B36" s="37" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="C36" s="28" t="s">
         <v>30</v>
@@ -11758,7 +11762,7 @@
         <v>253</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="F36" s="29"/>
       <c r="G36" s="29"/>
@@ -11773,10 +11777,10 @@
     </row>
     <row r="37" ht="23" customHeight="1" spans="1:15">
       <c r="A37" s="26" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="C37" s="31" t="s">
         <v>30</v>
@@ -11785,7 +11789,7 @@
         <v>253</v>
       </c>
       <c r="E37" s="32" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="F37" s="32"/>
       <c r="G37" s="29"/>
@@ -11800,10 +11804,10 @@
     </row>
     <row r="38" ht="23" customHeight="1" spans="1:15">
       <c r="A38" s="26" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="C38" s="31" t="s">
         <v>30</v>
@@ -11812,7 +11816,7 @@
         <v>253</v>
       </c>
       <c r="E38" s="32" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="F38" s="32"/>
       <c r="G38" s="29"/>
@@ -11827,10 +11831,10 @@
     </row>
     <row r="39" ht="23" customHeight="1" spans="1:15">
       <c r="A39" s="26" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="C39" s="31" t="s">
         <v>30</v>
@@ -11839,7 +11843,7 @@
         <v>576</v>
       </c>
       <c r="E39" s="29" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="F39" s="29" t="s">
         <v>750</v>
@@ -11857,7 +11861,7 @@
     <row r="40" ht="23" customHeight="1" spans="1:15">
       <c r="A40" s="26"/>
       <c r="B40" s="37" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="C40" s="28" t="s">
         <v>30</v>
@@ -11866,7 +11870,7 @@
         <v>363</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="F40" s="29"/>
       <c r="G40" s="29"/>

</xml_diff>